<commit_message>
add vote spread columns
</commit_message>
<xml_diff>
--- a/processed_data/joined.xlsx
+++ b/processed_data/joined.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X211"/>
+  <dimension ref="A1:AA211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -478,6 +478,21 @@
           <t>vote_change_ratio_gop</t>
         </is>
       </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>votespread_18_dem</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>votespread_19_dem</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>votespread_GAINdiff_dem</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -566,6 +581,15 @@
       <c r="X2">
         <v>1.04</v>
       </c>
+      <c r="Y2">
+        <v>65</v>
+      </c>
+      <c r="Z2">
+        <v>68</v>
+      </c>
+      <c r="AA2">
+        <v>3</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -654,6 +678,15 @@
       <c r="X3">
         <v>2.23</v>
       </c>
+      <c r="Y3">
+        <v>-287</v>
+      </c>
+      <c r="Z3">
+        <v>-213</v>
+      </c>
+      <c r="AA3">
+        <v>74</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -742,6 +775,15 @@
       <c r="X4">
         <v>0.37</v>
       </c>
+      <c r="Y4">
+        <v>148</v>
+      </c>
+      <c r="Z4">
+        <v>79</v>
+      </c>
+      <c r="AA4">
+        <v>-69</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -830,6 +872,15 @@
       <c r="X5">
         <v>0.46</v>
       </c>
+      <c r="Y5">
+        <v>348</v>
+      </c>
+      <c r="Z5">
+        <v>221</v>
+      </c>
+      <c r="AA5">
+        <v>-127</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -918,6 +969,15 @@
       <c r="X6">
         <v>0.23</v>
       </c>
+      <c r="Y6">
+        <v>383</v>
+      </c>
+      <c r="Z6">
+        <v>258</v>
+      </c>
+      <c r="AA6">
+        <v>-125</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1006,6 +1066,15 @@
       <c r="X7">
         <v>1.7</v>
       </c>
+      <c r="Y7">
+        <v>-317</v>
+      </c>
+      <c r="Z7">
+        <v>-270</v>
+      </c>
+      <c r="AA7">
+        <v>47</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1094,6 +1163,15 @@
       <c r="X8">
         <v>1.07</v>
       </c>
+      <c r="Y8">
+        <v>-44</v>
+      </c>
+      <c r="Z8">
+        <v>-39</v>
+      </c>
+      <c r="AA8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1182,6 +1260,15 @@
       <c r="X9">
         <v>0.37</v>
       </c>
+      <c r="Y9">
+        <v>484</v>
+      </c>
+      <c r="Z9">
+        <v>336</v>
+      </c>
+      <c r="AA9">
+        <v>-148</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1270,6 +1357,15 @@
       <c r="X10">
         <v>0.43</v>
       </c>
+      <c r="Y10">
+        <v>299</v>
+      </c>
+      <c r="Z10">
+        <v>210</v>
+      </c>
+      <c r="AA10">
+        <v>-89</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1358,6 +1454,15 @@
       <c r="X11">
         <v>0.55</v>
       </c>
+      <c r="Y11">
+        <v>259</v>
+      </c>
+      <c r="Z11">
+        <v>158</v>
+      </c>
+      <c r="AA11">
+        <v>-101</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1446,6 +1551,15 @@
       <c r="X12">
         <v>0.7</v>
       </c>
+      <c r="Y12">
+        <v>-18</v>
+      </c>
+      <c r="Z12">
+        <v>-24</v>
+      </c>
+      <c r="AA12">
+        <v>-6</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1534,6 +1648,15 @@
       <c r="X13">
         <v>-0.16</v>
       </c>
+      <c r="Y13">
+        <v>-28</v>
+      </c>
+      <c r="Z13">
+        <v>-71</v>
+      </c>
+      <c r="AA13">
+        <v>-43</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1622,6 +1745,15 @@
       <c r="X14">
         <v>0.27</v>
       </c>
+      <c r="Y14">
+        <v>-308</v>
+      </c>
+      <c r="Z14">
+        <v>-378</v>
+      </c>
+      <c r="AA14">
+        <v>-70</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1710,6 +1842,15 @@
       <c r="X15">
         <v>-0.5600000000000001</v>
       </c>
+      <c r="Y15">
+        <v>-243</v>
+      </c>
+      <c r="Z15">
+        <v>-268</v>
+      </c>
+      <c r="AA15">
+        <v>-25</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1798,6 +1939,15 @@
       <c r="X16">
         <v>-0.5600000000000001</v>
       </c>
+      <c r="Y16">
+        <v>-135</v>
+      </c>
+      <c r="Z16">
+        <v>-221</v>
+      </c>
+      <c r="AA16">
+        <v>-86</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1886,6 +2036,15 @@
       <c r="X17">
         <v>0.4</v>
       </c>
+      <c r="Y17">
+        <v>4</v>
+      </c>
+      <c r="Z17">
+        <v>-17</v>
+      </c>
+      <c r="AA17">
+        <v>-21</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1974,6 +2133,15 @@
       <c r="X18">
         <v>8</v>
       </c>
+      <c r="Y18">
+        <v>21</v>
+      </c>
+      <c r="Z18">
+        <v>35</v>
+      </c>
+      <c r="AA18">
+        <v>14</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2062,6 +2230,15 @@
       <c r="X19">
         <v>0.75</v>
       </c>
+      <c r="Y19">
+        <v>-131</v>
+      </c>
+      <c r="Z19">
+        <v>-129</v>
+      </c>
+      <c r="AA19">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2150,6 +2327,15 @@
       <c r="X20">
         <v>2.55</v>
       </c>
+      <c r="Y20">
+        <v>-60</v>
+      </c>
+      <c r="Z20">
+        <v>-43</v>
+      </c>
+      <c r="AA20">
+        <v>17</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2238,6 +2424,15 @@
       <c r="X21">
         <v>1.64</v>
       </c>
+      <c r="Y21">
+        <v>54</v>
+      </c>
+      <c r="Z21">
+        <v>31</v>
+      </c>
+      <c r="AA21">
+        <v>-23</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2326,6 +2521,15 @@
       <c r="X22">
         <v>0.51</v>
       </c>
+      <c r="Y22">
+        <v>75</v>
+      </c>
+      <c r="Z22">
+        <v>26</v>
+      </c>
+      <c r="AA22">
+        <v>-49</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2414,6 +2618,15 @@
       <c r="X23">
         <v>2.18</v>
       </c>
+      <c r="Y23">
+        <v>-2</v>
+      </c>
+      <c r="Z23">
+        <v>11</v>
+      </c>
+      <c r="AA23">
+        <v>13</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2502,6 +2715,15 @@
       <c r="X24">
         <v>3.08</v>
       </c>
+      <c r="Y24">
+        <v>-79</v>
+      </c>
+      <c r="Z24">
+        <v>-54</v>
+      </c>
+      <c r="AA24">
+        <v>25</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2590,6 +2812,15 @@
       <c r="X25">
         <v>1.25</v>
       </c>
+      <c r="Y25">
+        <v>-255</v>
+      </c>
+      <c r="Z25">
+        <v>-346</v>
+      </c>
+      <c r="AA25">
+        <v>-91</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2678,6 +2909,15 @@
       <c r="X26">
         <v>0.26</v>
       </c>
+      <c r="Y26">
+        <v>356</v>
+      </c>
+      <c r="Z26">
+        <v>376</v>
+      </c>
+      <c r="AA26">
+        <v>20</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2766,6 +3006,15 @@
       <c r="X27">
         <v>-1.2</v>
       </c>
+      <c r="Y27">
+        <v>324</v>
+      </c>
+      <c r="Z27">
+        <v>302</v>
+      </c>
+      <c r="AA27">
+        <v>-22</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2854,6 +3103,15 @@
       <c r="X28">
         <v>-0.39</v>
       </c>
+      <c r="Y28">
+        <v>-36</v>
+      </c>
+      <c r="Z28">
+        <v>-11</v>
+      </c>
+      <c r="AA28">
+        <v>25</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2942,6 +3200,15 @@
       <c r="X29">
         <v>0.01</v>
       </c>
+      <c r="Y29">
+        <v>461</v>
+      </c>
+      <c r="Z29">
+        <v>700</v>
+      </c>
+      <c r="AA29">
+        <v>239</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3030,6 +3297,15 @@
       <c r="X30">
         <v>0.18</v>
       </c>
+      <c r="Y30">
+        <v>-414</v>
+      </c>
+      <c r="Z30">
+        <v>-311</v>
+      </c>
+      <c r="AA30">
+        <v>103</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3118,6 +3394,15 @@
       <c r="X31">
         <v>-2.94</v>
       </c>
+      <c r="Y31">
+        <v>-148</v>
+      </c>
+      <c r="Z31">
+        <v>-85</v>
+      </c>
+      <c r="AA31">
+        <v>63</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3206,6 +3491,15 @@
       <c r="X32">
         <v>7</v>
       </c>
+      <c r="Y32">
+        <v>198</v>
+      </c>
+      <c r="Z32">
+        <v>186</v>
+      </c>
+      <c r="AA32">
+        <v>-12</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3294,6 +3588,15 @@
       <c r="X33">
         <v>0.51</v>
       </c>
+      <c r="Y33">
+        <v>-310</v>
+      </c>
+      <c r="Z33">
+        <v>-217</v>
+      </c>
+      <c r="AA33">
+        <v>93</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3382,6 +3685,15 @@
       <c r="X34">
         <v>-0.69</v>
       </c>
+      <c r="Y34">
+        <v>274</v>
+      </c>
+      <c r="Z34">
+        <v>301</v>
+      </c>
+      <c r="AA34">
+        <v>27</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -3470,6 +3782,15 @@
       <c r="X35">
         <v>0.17</v>
       </c>
+      <c r="Y35">
+        <v>75</v>
+      </c>
+      <c r="Z35">
+        <v>41</v>
+      </c>
+      <c r="AA35">
+        <v>-34</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -3558,6 +3879,15 @@
       <c r="X36">
         <v>-0.32</v>
       </c>
+      <c r="Y36">
+        <v>32</v>
+      </c>
+      <c r="Z36">
+        <v>-30</v>
+      </c>
+      <c r="AA36">
+        <v>-62</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -3646,6 +3976,15 @@
       <c r="X37">
         <v>0.97</v>
       </c>
+      <c r="Y37">
+        <v>-61</v>
+      </c>
+      <c r="Z37">
+        <v>-60</v>
+      </c>
+      <c r="AA37">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -3734,6 +4073,15 @@
       <c r="X38">
         <v>0.69</v>
       </c>
+      <c r="Y38">
+        <v>-623</v>
+      </c>
+      <c r="Z38">
+        <v>-601</v>
+      </c>
+      <c r="AA38">
+        <v>22</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -3822,6 +4170,15 @@
       <c r="X39">
         <v>26</v>
       </c>
+      <c r="Y39">
+        <v>-252</v>
+      </c>
+      <c r="Z39">
+        <v>-177</v>
+      </c>
+      <c r="AA39">
+        <v>75</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -3910,6 +4267,15 @@
       <c r="X40">
         <v>-5.4</v>
       </c>
+      <c r="Y40">
+        <v>-179</v>
+      </c>
+      <c r="Z40">
+        <v>-115</v>
+      </c>
+      <c r="AA40">
+        <v>64</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3998,6 +4364,15 @@
       <c r="X41">
         <v>8.199999999999999</v>
       </c>
+      <c r="Y41">
+        <v>30</v>
+      </c>
+      <c r="Z41">
+        <v>-6</v>
+      </c>
+      <c r="AA41">
+        <v>-36</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4086,6 +4461,15 @@
       <c r="X42">
         <v>1.35</v>
       </c>
+      <c r="Y42">
+        <v>40</v>
+      </c>
+      <c r="Z42">
+        <v>18</v>
+      </c>
+      <c r="AA42">
+        <v>-22</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4174,6 +4558,15 @@
       <c r="X43">
         <v>0.59</v>
       </c>
+      <c r="Y43">
+        <v>-46</v>
+      </c>
+      <c r="Z43">
+        <v>63</v>
+      </c>
+      <c r="AA43">
+        <v>109</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4262,6 +4655,15 @@
       <c r="X44">
         <v>0.7</v>
       </c>
+      <c r="Y44">
+        <v>-98</v>
+      </c>
+      <c r="Z44">
+        <v>-64</v>
+      </c>
+      <c r="AA44">
+        <v>34</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -4350,6 +4752,15 @@
       <c r="X45">
         <v>1.02</v>
       </c>
+      <c r="Y45">
+        <v>317</v>
+      </c>
+      <c r="Z45">
+        <v>320</v>
+      </c>
+      <c r="AA45">
+        <v>3</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -4438,6 +4849,15 @@
       <c r="X46">
         <v>0.47</v>
       </c>
+      <c r="Y46">
+        <v>104</v>
+      </c>
+      <c r="Z46">
+        <v>86</v>
+      </c>
+      <c r="AA46">
+        <v>-18</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -4526,6 +4946,15 @@
       <c r="X47">
         <v>0.91</v>
       </c>
+      <c r="Y47">
+        <v>308</v>
+      </c>
+      <c r="Z47">
+        <v>284</v>
+      </c>
+      <c r="AA47">
+        <v>-24</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -4614,6 +5043,15 @@
       <c r="X48">
         <v>1.36</v>
       </c>
+      <c r="Y48">
+        <v>140</v>
+      </c>
+      <c r="Z48">
+        <v>178</v>
+      </c>
+      <c r="AA48">
+        <v>38</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -4702,6 +5140,15 @@
       <c r="X49">
         <v>1.01</v>
       </c>
+      <c r="Y49">
+        <v>285</v>
+      </c>
+      <c r="Z49">
+        <v>287</v>
+      </c>
+      <c r="AA49">
+        <v>2</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -4790,6 +5237,15 @@
       <c r="X50">
         <v>1.59</v>
       </c>
+      <c r="Y50">
+        <v>129</v>
+      </c>
+      <c r="Z50">
+        <v>216</v>
+      </c>
+      <c r="AA50">
+        <v>87</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -4878,6 +5334,15 @@
       <c r="X51">
         <v>1.39</v>
       </c>
+      <c r="Y51">
+        <v>124</v>
+      </c>
+      <c r="Z51">
+        <v>176</v>
+      </c>
+      <c r="AA51">
+        <v>52</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -4966,6 +5431,15 @@
       <c r="X52">
         <v>0.82</v>
       </c>
+      <c r="Y52">
+        <v>308</v>
+      </c>
+      <c r="Z52">
+        <v>271</v>
+      </c>
+      <c r="AA52">
+        <v>-37</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -5054,6 +5528,15 @@
       <c r="X53">
         <v>1.01</v>
       </c>
+      <c r="Y53">
+        <v>175</v>
+      </c>
+      <c r="Z53">
+        <v>180</v>
+      </c>
+      <c r="AA53">
+        <v>5</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -5142,6 +5625,15 @@
       <c r="X54">
         <v>1.31</v>
       </c>
+      <c r="Y54">
+        <v>186</v>
+      </c>
+      <c r="Z54">
+        <v>230</v>
+      </c>
+      <c r="AA54">
+        <v>44</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -5230,6 +5722,15 @@
       <c r="X55">
         <v>1.75</v>
       </c>
+      <c r="Y55">
+        <v>73</v>
+      </c>
+      <c r="Z55">
+        <v>146</v>
+      </c>
+      <c r="AA55">
+        <v>73</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -5318,6 +5819,15 @@
       <c r="X56">
         <v>0.94</v>
       </c>
+      <c r="Y56">
+        <v>239</v>
+      </c>
+      <c r="Z56">
+        <v>232</v>
+      </c>
+      <c r="AA56">
+        <v>-7</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -5406,6 +5916,15 @@
       <c r="X57">
         <v>0.72</v>
       </c>
+      <c r="Y57">
+        <v>265</v>
+      </c>
+      <c r="Z57">
+        <v>208</v>
+      </c>
+      <c r="AA57">
+        <v>-57</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -5494,6 +6013,15 @@
       <c r="X58">
         <v>0.77</v>
       </c>
+      <c r="Y58">
+        <v>349</v>
+      </c>
+      <c r="Z58">
+        <v>263</v>
+      </c>
+      <c r="AA58">
+        <v>-86</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -5582,6 +6110,15 @@
       <c r="X59">
         <v>0.9300000000000001</v>
       </c>
+      <c r="Y59">
+        <v>277</v>
+      </c>
+      <c r="Z59">
+        <v>260</v>
+      </c>
+      <c r="AA59">
+        <v>-17</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -5670,6 +6207,15 @@
       <c r="X60">
         <v>0.77</v>
       </c>
+      <c r="Y60">
+        <v>405</v>
+      </c>
+      <c r="Z60">
+        <v>340</v>
+      </c>
+      <c r="AA60">
+        <v>-65</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -5758,6 +6304,15 @@
       <c r="X61">
         <v>1.41</v>
       </c>
+      <c r="Y61">
+        <v>40</v>
+      </c>
+      <c r="Z61">
+        <v>93</v>
+      </c>
+      <c r="AA61">
+        <v>53</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -5846,6 +6401,15 @@
       <c r="X62">
         <v>1.44</v>
       </c>
+      <c r="Y62">
+        <v>148</v>
+      </c>
+      <c r="Z62">
+        <v>196</v>
+      </c>
+      <c r="AA62">
+        <v>48</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -5934,6 +6498,15 @@
       <c r="X63">
         <v>1.15</v>
       </c>
+      <c r="Y63">
+        <v>211</v>
+      </c>
+      <c r="Z63">
+        <v>258</v>
+      </c>
+      <c r="AA63">
+        <v>47</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -6022,6 +6595,15 @@
       <c r="X64">
         <v>0.8</v>
       </c>
+      <c r="Y64">
+        <v>257</v>
+      </c>
+      <c r="Z64">
+        <v>203</v>
+      </c>
+      <c r="AA64">
+        <v>-54</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -6110,6 +6692,15 @@
       <c r="X65">
         <v>0.88</v>
       </c>
+      <c r="Y65">
+        <v>-45</v>
+      </c>
+      <c r="Z65">
+        <v>-62</v>
+      </c>
+      <c r="AA65">
+        <v>-17</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -6198,6 +6789,15 @@
       <c r="X66">
         <v>0.7</v>
       </c>
+      <c r="Y66">
+        <v>295</v>
+      </c>
+      <c r="Z66">
+        <v>230</v>
+      </c>
+      <c r="AA66">
+        <v>-65</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -6286,6 +6886,15 @@
       <c r="X67">
         <v>0.88</v>
       </c>
+      <c r="Y67">
+        <v>304</v>
+      </c>
+      <c r="Z67">
+        <v>271</v>
+      </c>
+      <c r="AA67">
+        <v>-33</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -6374,6 +6983,15 @@
       <c r="X68">
         <v>0.67</v>
       </c>
+      <c r="Y68">
+        <v>159</v>
+      </c>
+      <c r="Z68">
+        <v>62</v>
+      </c>
+      <c r="AA68">
+        <v>-97</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -6462,6 +7080,15 @@
       <c r="X69">
         <v>1.03</v>
       </c>
+      <c r="Y69">
+        <v>171</v>
+      </c>
+      <c r="Z69">
+        <v>178</v>
+      </c>
+      <c r="AA69">
+        <v>7</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -6550,6 +7177,15 @@
       <c r="X70">
         <v>0.89</v>
       </c>
+      <c r="Y70">
+        <v>169</v>
+      </c>
+      <c r="Z70">
+        <v>156</v>
+      </c>
+      <c r="AA70">
+        <v>-13</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -6638,6 +7274,15 @@
       <c r="X71">
         <v>0.83</v>
       </c>
+      <c r="Y71">
+        <v>370</v>
+      </c>
+      <c r="Z71">
+        <v>328</v>
+      </c>
+      <c r="AA71">
+        <v>-42</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -6726,6 +7371,15 @@
       <c r="X72">
         <v>1.08</v>
       </c>
+      <c r="Y72">
+        <v>-2</v>
+      </c>
+      <c r="Z72">
+        <v>13</v>
+      </c>
+      <c r="AA72">
+        <v>15</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -6814,6 +7468,15 @@
       <c r="X73">
         <v>1.12</v>
       </c>
+      <c r="Y73">
+        <v>135</v>
+      </c>
+      <c r="Z73">
+        <v>170</v>
+      </c>
+      <c r="AA73">
+        <v>35</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -6902,6 +7565,15 @@
       <c r="X74">
         <v>0.9300000000000001</v>
       </c>
+      <c r="Y74">
+        <v>200</v>
+      </c>
+      <c r="Z74">
+        <v>180</v>
+      </c>
+      <c r="AA74">
+        <v>-20</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -6990,6 +7662,15 @@
       <c r="X75">
         <v>0.73</v>
       </c>
+      <c r="Y75">
+        <v>326</v>
+      </c>
+      <c r="Z75">
+        <v>243</v>
+      </c>
+      <c r="AA75">
+        <v>-83</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -7078,6 +7759,15 @@
       <c r="X76">
         <v>0.75</v>
       </c>
+      <c r="Y76">
+        <v>209</v>
+      </c>
+      <c r="Z76">
+        <v>170</v>
+      </c>
+      <c r="AA76">
+        <v>-39</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -7166,6 +7856,15 @@
       <c r="X77">
         <v>1.34</v>
       </c>
+      <c r="Y77">
+        <v>14</v>
+      </c>
+      <c r="Z77">
+        <v>110</v>
+      </c>
+      <c r="AA77">
+        <v>96</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -7254,6 +7953,15 @@
       <c r="X78">
         <v>1.24</v>
       </c>
+      <c r="Y78">
+        <v>69</v>
+      </c>
+      <c r="Z78">
+        <v>99</v>
+      </c>
+      <c r="AA78">
+        <v>30</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -7342,6 +8050,15 @@
       <c r="X79">
         <v>1.43</v>
       </c>
+      <c r="Y79">
+        <v>-13</v>
+      </c>
+      <c r="Z79">
+        <v>37</v>
+      </c>
+      <c r="AA79">
+        <v>50</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -7430,6 +8147,15 @@
       <c r="X80">
         <v>1.07</v>
       </c>
+      <c r="Y80">
+        <v>95</v>
+      </c>
+      <c r="Z80">
+        <v>130</v>
+      </c>
+      <c r="AA80">
+        <v>35</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -7518,6 +8244,15 @@
       <c r="X81">
         <v>0.79</v>
       </c>
+      <c r="Y81">
+        <v>291</v>
+      </c>
+      <c r="Z81">
+        <v>213</v>
+      </c>
+      <c r="AA81">
+        <v>-78</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -7606,6 +8341,15 @@
       <c r="X82">
         <v>0.84</v>
       </c>
+      <c r="Y82">
+        <v>295</v>
+      </c>
+      <c r="Z82">
+        <v>240</v>
+      </c>
+      <c r="AA82">
+        <v>-55</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -7694,6 +8438,15 @@
       <c r="X83">
         <v>0.74</v>
       </c>
+      <c r="Y83">
+        <v>227</v>
+      </c>
+      <c r="Z83">
+        <v>154</v>
+      </c>
+      <c r="AA83">
+        <v>-73</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -7782,6 +8535,15 @@
       <c r="X84">
         <v>1.06</v>
       </c>
+      <c r="Y84">
+        <v>331</v>
+      </c>
+      <c r="Z84">
+        <v>354</v>
+      </c>
+      <c r="AA84">
+        <v>23</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -7870,6 +8632,15 @@
       <c r="X85">
         <v>0.85</v>
       </c>
+      <c r="Y85">
+        <v>224</v>
+      </c>
+      <c r="Z85">
+        <v>187</v>
+      </c>
+      <c r="AA85">
+        <v>-37</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -7958,6 +8729,15 @@
       <c r="X86">
         <v>1.35</v>
       </c>
+      <c r="Y86">
+        <v>-215</v>
+      </c>
+      <c r="Z86">
+        <v>-146</v>
+      </c>
+      <c r="AA86">
+        <v>69</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -8046,6 +8826,15 @@
       <c r="X87">
         <v>1.52</v>
       </c>
+      <c r="Y87">
+        <v>-145</v>
+      </c>
+      <c r="Z87">
+        <v>-60</v>
+      </c>
+      <c r="AA87">
+        <v>85</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -8134,6 +8923,15 @@
       <c r="X88">
         <v>1.41</v>
       </c>
+      <c r="Y88">
+        <v>-242</v>
+      </c>
+      <c r="Z88">
+        <v>-161</v>
+      </c>
+      <c r="AA88">
+        <v>81</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -8222,6 +9020,15 @@
       <c r="X89">
         <v>1.82</v>
       </c>
+      <c r="Y89">
+        <v>-576</v>
+      </c>
+      <c r="Z89">
+        <v>-385</v>
+      </c>
+      <c r="AA89">
+        <v>191</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -8310,6 +9117,15 @@
       <c r="X90">
         <v>0.86</v>
       </c>
+      <c r="Y90">
+        <v>339</v>
+      </c>
+      <c r="Z90">
+        <v>286</v>
+      </c>
+      <c r="AA90">
+        <v>-53</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -8398,6 +9214,15 @@
       <c r="X91">
         <v>0.96</v>
       </c>
+      <c r="Y91">
+        <v>524</v>
+      </c>
+      <c r="Z91">
+        <v>501</v>
+      </c>
+      <c r="AA91">
+        <v>-23</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -8486,6 +9311,15 @@
       <c r="X92">
         <v>0.85</v>
       </c>
+      <c r="Y92">
+        <v>244</v>
+      </c>
+      <c r="Z92">
+        <v>179</v>
+      </c>
+      <c r="AA92">
+        <v>-65</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -8574,6 +9408,15 @@
       <c r="X93">
         <v>1.78</v>
       </c>
+      <c r="Y93">
+        <v>-22</v>
+      </c>
+      <c r="Z93">
+        <v>129</v>
+      </c>
+      <c r="AA93">
+        <v>151</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -8662,6 +9505,15 @@
       <c r="X94">
         <v>1.64</v>
       </c>
+      <c r="Y94">
+        <v>-529</v>
+      </c>
+      <c r="Z94">
+        <v>-346</v>
+      </c>
+      <c r="AA94">
+        <v>183</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -8750,6 +9602,15 @@
       <c r="X95">
         <v>0.31</v>
       </c>
+      <c r="Y95">
+        <v>274</v>
+      </c>
+      <c r="Z95">
+        <v>153</v>
+      </c>
+      <c r="AA95">
+        <v>-121</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -8838,6 +9699,15 @@
       <c r="X96">
         <v>0.77</v>
       </c>
+      <c r="Y96">
+        <v>-138</v>
+      </c>
+      <c r="Z96">
+        <v>-154</v>
+      </c>
+      <c r="AA96">
+        <v>-16</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -8926,6 +9796,15 @@
       <c r="X97">
         <v>0.8</v>
       </c>
+      <c r="Y97">
+        <v>-83</v>
+      </c>
+      <c r="Z97">
+        <v>-87</v>
+      </c>
+      <c r="AA97">
+        <v>-4</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -9014,6 +9893,15 @@
       <c r="X98">
         <v>0.21</v>
       </c>
+      <c r="Y98">
+        <v>50</v>
+      </c>
+      <c r="Z98">
+        <v>0</v>
+      </c>
+      <c r="AA98">
+        <v>-50</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -9102,6 +9990,15 @@
       <c r="X99">
         <v>0.58</v>
       </c>
+      <c r="Y99">
+        <v>-7</v>
+      </c>
+      <c r="Z99">
+        <v>-15</v>
+      </c>
+      <c r="AA99">
+        <v>-8</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -9190,6 +10087,15 @@
       <c r="X100">
         <v>0.49</v>
       </c>
+      <c r="Y100">
+        <v>-93</v>
+      </c>
+      <c r="Z100">
+        <v>-121</v>
+      </c>
+      <c r="AA100">
+        <v>-28</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -9278,6 +10184,15 @@
       <c r="X101">
         <v>0.22</v>
       </c>
+      <c r="Y101">
+        <v>29</v>
+      </c>
+      <c r="Z101">
+        <v>0</v>
+      </c>
+      <c r="AA101">
+        <v>-29</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -9366,6 +10281,15 @@
       <c r="X102">
         <v>0.21</v>
       </c>
+      <c r="Y102">
+        <v>155</v>
+      </c>
+      <c r="Z102">
+        <v>44</v>
+      </c>
+      <c r="AA102">
+        <v>-111</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -9454,6 +10378,15 @@
       <c r="X103">
         <v>0.64</v>
       </c>
+      <c r="Y103">
+        <v>-135</v>
+      </c>
+      <c r="Z103">
+        <v>-181</v>
+      </c>
+      <c r="AA103">
+        <v>-46</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -9542,6 +10475,15 @@
       <c r="X104">
         <v>0.38</v>
       </c>
+      <c r="Y104">
+        <v>123</v>
+      </c>
+      <c r="Z104">
+        <v>58</v>
+      </c>
+      <c r="AA104">
+        <v>-65</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -9630,6 +10572,15 @@
       <c r="X105">
         <v>0.42</v>
       </c>
+      <c r="Y105">
+        <v>-5</v>
+      </c>
+      <c r="Z105">
+        <v>-43</v>
+      </c>
+      <c r="AA105">
+        <v>-38</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -9718,6 +10669,15 @@
       <c r="X106">
         <v>0.31</v>
       </c>
+      <c r="Y106">
+        <v>-27</v>
+      </c>
+      <c r="Z106">
+        <v>-106</v>
+      </c>
+      <c r="AA106">
+        <v>-79</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -9806,6 +10766,15 @@
       <c r="X107">
         <v>0.98</v>
       </c>
+      <c r="Y107">
+        <v>-41</v>
+      </c>
+      <c r="Z107">
+        <v>-42</v>
+      </c>
+      <c r="AA107">
+        <v>-1</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -9894,6 +10863,15 @@
       <c r="X108">
         <v>0.42</v>
       </c>
+      <c r="Y108">
+        <v>29</v>
+      </c>
+      <c r="Z108">
+        <v>18</v>
+      </c>
+      <c r="AA108">
+        <v>-11</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -9982,6 +10960,15 @@
       <c r="X109">
         <v>6</v>
       </c>
+      <c r="Y109">
+        <v>-31</v>
+      </c>
+      <c r="Z109">
+        <v>-26</v>
+      </c>
+      <c r="AA109">
+        <v>5</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -10070,6 +11057,15 @@
       <c r="X110">
         <v>1.45</v>
       </c>
+      <c r="Y110">
+        <v>-81</v>
+      </c>
+      <c r="Z110">
+        <v>-76</v>
+      </c>
+      <c r="AA110">
+        <v>5</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -10158,6 +11154,15 @@
       <c r="X111">
         <v>0.14</v>
       </c>
+      <c r="Y111">
+        <v>85</v>
+      </c>
+      <c r="Z111">
+        <v>-21</v>
+      </c>
+      <c r="AA111">
+        <v>-106</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -10246,6 +11251,15 @@
       <c r="X112">
         <v>0.17</v>
       </c>
+      <c r="Y112">
+        <v>374</v>
+      </c>
+      <c r="Z112">
+        <v>151</v>
+      </c>
+      <c r="AA112">
+        <v>-223</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -10334,6 +11348,15 @@
       <c r="X113">
         <v>0.51</v>
       </c>
+      <c r="Y113">
+        <v>-184</v>
+      </c>
+      <c r="Z113">
+        <v>-244</v>
+      </c>
+      <c r="AA113">
+        <v>-60</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -10422,6 +11445,15 @@
       <c r="X114">
         <v>0.05</v>
       </c>
+      <c r="Y114">
+        <v>179</v>
+      </c>
+      <c r="Z114">
+        <v>-83</v>
+      </c>
+      <c r="AA114">
+        <v>-262</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -10510,6 +11542,15 @@
       <c r="X115">
         <v>0.47</v>
       </c>
+      <c r="Y115">
+        <v>558</v>
+      </c>
+      <c r="Z115">
+        <v>455</v>
+      </c>
+      <c r="AA115">
+        <v>-103</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -10598,6 +11639,15 @@
       <c r="X116">
         <v>0.3</v>
       </c>
+      <c r="Y116">
+        <v>129</v>
+      </c>
+      <c r="Z116">
+        <v>70</v>
+      </c>
+      <c r="AA116">
+        <v>-59</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -10686,6 +11736,15 @@
       <c r="X117">
         <v>0.88</v>
       </c>
+      <c r="Y117">
+        <v>-283</v>
+      </c>
+      <c r="Z117">
+        <v>-297</v>
+      </c>
+      <c r="AA117">
+        <v>-14</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -10774,6 +11833,15 @@
       <c r="X118">
         <v>0.49</v>
       </c>
+      <c r="Y118">
+        <v>69</v>
+      </c>
+      <c r="Z118">
+        <v>6</v>
+      </c>
+      <c r="AA118">
+        <v>-63</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -10862,6 +11930,15 @@
       <c r="X119">
         <v>0.54</v>
       </c>
+      <c r="Y119">
+        <v>50</v>
+      </c>
+      <c r="Z119">
+        <v>-4</v>
+      </c>
+      <c r="AA119">
+        <v>-54</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -10950,6 +12027,15 @@
       <c r="X120">
         <v>0.8</v>
       </c>
+      <c r="Y120">
+        <v>-502</v>
+      </c>
+      <c r="Z120">
+        <v>-562</v>
+      </c>
+      <c r="AA120">
+        <v>-60</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -11038,6 +12124,15 @@
       <c r="X121">
         <v>0.27</v>
       </c>
+      <c r="Y121">
+        <v>67</v>
+      </c>
+      <c r="Z121">
+        <v>-19</v>
+      </c>
+      <c r="AA121">
+        <v>-86</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -11126,6 +12221,15 @@
       <c r="X122">
         <v>0.23</v>
       </c>
+      <c r="Y122">
+        <v>357</v>
+      </c>
+      <c r="Z122">
+        <v>205</v>
+      </c>
+      <c r="AA122">
+        <v>-152</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -11214,6 +12318,15 @@
       <c r="X123">
         <v>0.27</v>
       </c>
+      <c r="Y123">
+        <v>161</v>
+      </c>
+      <c r="Z123">
+        <v>9</v>
+      </c>
+      <c r="AA123">
+        <v>-152</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -11302,6 +12415,15 @@
       <c r="X124">
         <v>0.42</v>
       </c>
+      <c r="Y124">
+        <v>68</v>
+      </c>
+      <c r="Z124">
+        <v>2</v>
+      </c>
+      <c r="AA124">
+        <v>-66</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -11390,6 +12512,15 @@
       <c r="X125">
         <v>0.31</v>
       </c>
+      <c r="Y125">
+        <v>317</v>
+      </c>
+      <c r="Z125">
+        <v>244</v>
+      </c>
+      <c r="AA125">
+        <v>-73</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -11478,6 +12609,15 @@
       <c r="X126">
         <v>0.07000000000000001</v>
       </c>
+      <c r="Y126">
+        <v>457</v>
+      </c>
+      <c r="Z126">
+        <v>319</v>
+      </c>
+      <c r="AA126">
+        <v>-138</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -11566,6 +12706,15 @@
       <c r="X127">
         <v>0.39</v>
       </c>
+      <c r="Y127">
+        <v>57</v>
+      </c>
+      <c r="Z127">
+        <v>37</v>
+      </c>
+      <c r="AA127">
+        <v>-20</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -11654,6 +12803,15 @@
       <c r="X128">
         <v>0.67</v>
       </c>
+      <c r="Y128">
+        <v>17</v>
+      </c>
+      <c r="Z128">
+        <v>-34</v>
+      </c>
+      <c r="AA128">
+        <v>-51</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -11742,6 +12900,15 @@
       <c r="X129">
         <v>0.07000000000000001</v>
       </c>
+      <c r="Y129">
+        <v>694</v>
+      </c>
+      <c r="Z129">
+        <v>434</v>
+      </c>
+      <c r="AA129">
+        <v>-260</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -11830,6 +12997,15 @@
       <c r="X130">
         <v>0.49</v>
       </c>
+      <c r="Y130">
+        <v>6</v>
+      </c>
+      <c r="Z130">
+        <v>-49</v>
+      </c>
+      <c r="AA130">
+        <v>-55</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -11918,6 +13094,15 @@
       <c r="X131">
         <v>0.9</v>
       </c>
+      <c r="Y131">
+        <v>-14</v>
+      </c>
+      <c r="Z131">
+        <v>-32</v>
+      </c>
+      <c r="AA131">
+        <v>-18</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -12006,6 +13191,15 @@
       <c r="X132">
         <v>0.19</v>
       </c>
+      <c r="Y132">
+        <v>302</v>
+      </c>
+      <c r="Z132">
+        <v>43</v>
+      </c>
+      <c r="AA132">
+        <v>-259</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -12094,6 +13288,15 @@
       <c r="X133">
         <v>0.23</v>
       </c>
+      <c r="Y133">
+        <v>346</v>
+      </c>
+      <c r="Z133">
+        <v>66</v>
+      </c>
+      <c r="AA133">
+        <v>-280</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -12182,6 +13385,15 @@
       <c r="X134">
         <v>0.09</v>
       </c>
+      <c r="Y134">
+        <v>60</v>
+      </c>
+      <c r="Z134">
+        <v>-42</v>
+      </c>
+      <c r="AA134">
+        <v>-102</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -12270,6 +13482,15 @@
       <c r="X135">
         <v>0.16</v>
       </c>
+      <c r="Y135">
+        <v>146</v>
+      </c>
+      <c r="Z135">
+        <v>-4</v>
+      </c>
+      <c r="AA135">
+        <v>-150</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -12358,6 +13579,15 @@
       <c r="X136">
         <v>0.22</v>
       </c>
+      <c r="Y136">
+        <v>768</v>
+      </c>
+      <c r="Z136">
+        <v>486</v>
+      </c>
+      <c r="AA136">
+        <v>-282</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -12446,6 +13676,15 @@
       <c r="X137">
         <v>0.31</v>
       </c>
+      <c r="Y137">
+        <v>30</v>
+      </c>
+      <c r="Z137">
+        <v>-45</v>
+      </c>
+      <c r="AA137">
+        <v>-75</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -12534,6 +13773,15 @@
       <c r="X138">
         <v>0.18</v>
       </c>
+      <c r="Y138">
+        <v>288</v>
+      </c>
+      <c r="Z138">
+        <v>154</v>
+      </c>
+      <c r="AA138">
+        <v>-134</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -12622,6 +13870,15 @@
       <c r="X139">
         <v>0.24</v>
       </c>
+      <c r="Y139">
+        <v>174</v>
+      </c>
+      <c r="Z139">
+        <v>-71</v>
+      </c>
+      <c r="AA139">
+        <v>-245</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -12710,6 +13967,15 @@
       <c r="X140">
         <v>0.65</v>
       </c>
+      <c r="Y140">
+        <v>25</v>
+      </c>
+      <c r="Z140">
+        <v>-111</v>
+      </c>
+      <c r="AA140">
+        <v>-136</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -12798,6 +14064,15 @@
       <c r="X141">
         <v>0.62</v>
       </c>
+      <c r="Y141">
+        <v>36</v>
+      </c>
+      <c r="Z141">
+        <v>22</v>
+      </c>
+      <c r="AA141">
+        <v>-14</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -12886,6 +14161,15 @@
       <c r="X142">
         <v>0.16</v>
       </c>
+      <c r="Y142">
+        <v>6</v>
+      </c>
+      <c r="Z142">
+        <v>-113</v>
+      </c>
+      <c r="AA142">
+        <v>-119</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -12974,6 +14258,15 @@
       <c r="X143">
         <v>0.22</v>
       </c>
+      <c r="Y143">
+        <v>82</v>
+      </c>
+      <c r="Z143">
+        <v>-125</v>
+      </c>
+      <c r="AA143">
+        <v>-207</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -13062,6 +14355,15 @@
       <c r="X144">
         <v>0.16</v>
       </c>
+      <c r="Y144">
+        <v>121</v>
+      </c>
+      <c r="Z144">
+        <v>16</v>
+      </c>
+      <c r="AA144">
+        <v>-105</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -13150,6 +14452,15 @@
       <c r="X145">
         <v>0.87</v>
       </c>
+      <c r="Y145">
+        <v>-145</v>
+      </c>
+      <c r="Z145">
+        <v>-150</v>
+      </c>
+      <c r="AA145">
+        <v>-5</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -13238,6 +14549,15 @@
       <c r="X146">
         <v>0.13</v>
       </c>
+      <c r="Y146">
+        <v>26</v>
+      </c>
+      <c r="Z146">
+        <v>-20</v>
+      </c>
+      <c r="AA146">
+        <v>-46</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -13326,6 +14646,15 @@
       <c r="X147">
         <v>0.08</v>
       </c>
+      <c r="Y147">
+        <v>177</v>
+      </c>
+      <c r="Z147">
+        <v>-9</v>
+      </c>
+      <c r="AA147">
+        <v>-186</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -13414,6 +14743,15 @@
       <c r="X148">
         <v>0.87</v>
       </c>
+      <c r="Y148">
+        <v>37</v>
+      </c>
+      <c r="Z148">
+        <v>28</v>
+      </c>
+      <c r="AA148">
+        <v>-9</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -13502,6 +14840,15 @@
       <c r="X149">
         <v>0.74</v>
       </c>
+      <c r="Y149">
+        <v>-413</v>
+      </c>
+      <c r="Z149">
+        <v>-481</v>
+      </c>
+      <c r="AA149">
+        <v>-68</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -13590,6 +14937,15 @@
       <c r="X150">
         <v>0.02</v>
       </c>
+      <c r="Y150">
+        <v>274</v>
+      </c>
+      <c r="Z150">
+        <v>230</v>
+      </c>
+      <c r="AA150">
+        <v>-44</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -13678,6 +15034,15 @@
       <c r="X151">
         <v>-0.58</v>
       </c>
+      <c r="Y151">
+        <v>157</v>
+      </c>
+      <c r="Z151">
+        <v>138</v>
+      </c>
+      <c r="AA151">
+        <v>-19</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -13768,6 +15133,15 @@
       <c r="X152">
         <v>0</v>
       </c>
+      <c r="Y152">
+        <v>75</v>
+      </c>
+      <c r="Z152">
+        <v>29</v>
+      </c>
+      <c r="AA152">
+        <v>-46</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -13856,6 +15230,15 @@
       <c r="X153">
         <v>0.32</v>
       </c>
+      <c r="Y153">
+        <v>-43</v>
+      </c>
+      <c r="Z153">
+        <v>-88</v>
+      </c>
+      <c r="AA153">
+        <v>-45</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -13944,6 +15327,15 @@
       <c r="X154">
         <v>1.04</v>
       </c>
+      <c r="Y154">
+        <v>-123</v>
+      </c>
+      <c r="Z154">
+        <v>-121</v>
+      </c>
+      <c r="AA154">
+        <v>2</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -14032,6 +15424,15 @@
       <c r="X155">
         <v>0.67</v>
       </c>
+      <c r="Y155">
+        <v>5</v>
+      </c>
+      <c r="Z155">
+        <v>-4</v>
+      </c>
+      <c r="AA155">
+        <v>-9</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -14120,6 +15521,15 @@
       <c r="X156">
         <v>0.26</v>
       </c>
+      <c r="Y156">
+        <v>169</v>
+      </c>
+      <c r="Z156">
+        <v>116</v>
+      </c>
+      <c r="AA156">
+        <v>-53</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -14208,6 +15618,15 @@
       <c r="X157">
         <v>0.22</v>
       </c>
+      <c r="Y157">
+        <v>-61</v>
+      </c>
+      <c r="Z157">
+        <v>-68</v>
+      </c>
+      <c r="AA157">
+        <v>-7</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -14296,6 +15715,15 @@
       <c r="X158">
         <v>0.72</v>
       </c>
+      <c r="Y158">
+        <v>-55</v>
+      </c>
+      <c r="Z158">
+        <v>-71</v>
+      </c>
+      <c r="AA158">
+        <v>-16</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -14384,6 +15812,15 @@
       <c r="X159">
         <v>0.33</v>
       </c>
+      <c r="Y159">
+        <v>30</v>
+      </c>
+      <c r="Z159">
+        <v>-16</v>
+      </c>
+      <c r="AA159">
+        <v>-46</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -14472,6 +15909,15 @@
       <c r="X160">
         <v>0.25</v>
       </c>
+      <c r="Y160">
+        <v>194</v>
+      </c>
+      <c r="Z160">
+        <v>106</v>
+      </c>
+      <c r="AA160">
+        <v>-88</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -14560,6 +16006,15 @@
       <c r="X161">
         <v>0.45</v>
       </c>
+      <c r="Y161">
+        <v>294</v>
+      </c>
+      <c r="Z161">
+        <v>208</v>
+      </c>
+      <c r="AA161">
+        <v>-86</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -14648,6 +16103,15 @@
       <c r="X162">
         <v>0.89</v>
       </c>
+      <c r="Y162">
+        <v>71</v>
+      </c>
+      <c r="Z162">
+        <v>63</v>
+      </c>
+      <c r="AA162">
+        <v>-8</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -14736,6 +16200,15 @@
       <c r="X163">
         <v>0.22</v>
       </c>
+      <c r="Y163">
+        <v>382</v>
+      </c>
+      <c r="Z163">
+        <v>253</v>
+      </c>
+      <c r="AA163">
+        <v>-129</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -14824,6 +16297,15 @@
       <c r="X164">
         <v>1.12</v>
       </c>
+      <c r="Y164">
+        <v>-221</v>
+      </c>
+      <c r="Z164">
+        <v>-189</v>
+      </c>
+      <c r="AA164">
+        <v>32</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -14912,6 +16394,15 @@
       <c r="X165">
         <v>2.44</v>
       </c>
+      <c r="Y165">
+        <v>-510</v>
+      </c>
+      <c r="Z165">
+        <v>-389</v>
+      </c>
+      <c r="AA165">
+        <v>121</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -15000,6 +16491,15 @@
       <c r="X166">
         <v>1.19</v>
       </c>
+      <c r="Y166">
+        <v>-361</v>
+      </c>
+      <c r="Z166">
+        <v>-314</v>
+      </c>
+      <c r="AA166">
+        <v>47</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -15088,6 +16588,15 @@
       <c r="X167">
         <v>0.52</v>
       </c>
+      <c r="Y167">
+        <v>378</v>
+      </c>
+      <c r="Z167">
+        <v>241</v>
+      </c>
+      <c r="AA167">
+        <v>-137</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -15176,6 +16685,15 @@
       <c r="X168">
         <v>0.41</v>
       </c>
+      <c r="Y168">
+        <v>217</v>
+      </c>
+      <c r="Z168">
+        <v>137</v>
+      </c>
+      <c r="AA168">
+        <v>-80</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -15264,6 +16782,15 @@
       <c r="X169">
         <v>0.51</v>
       </c>
+      <c r="Y169">
+        <v>256</v>
+      </c>
+      <c r="Z169">
+        <v>208</v>
+      </c>
+      <c r="AA169">
+        <v>-48</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -15352,6 +16879,15 @@
       <c r="X170">
         <v>7.15</v>
       </c>
+      <c r="Y170">
+        <v>-1094</v>
+      </c>
+      <c r="Z170">
+        <v>-713</v>
+      </c>
+      <c r="AA170">
+        <v>381</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -15440,6 +16976,15 @@
       <c r="X171">
         <v>4.85</v>
       </c>
+      <c r="Y171">
+        <v>-1064</v>
+      </c>
+      <c r="Z171">
+        <v>-829</v>
+      </c>
+      <c r="AA171">
+        <v>235</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -15528,6 +17073,15 @@
       <c r="X172">
         <v>6.24</v>
       </c>
+      <c r="Y172">
+        <v>-1170</v>
+      </c>
+      <c r="Z172">
+        <v>-866</v>
+      </c>
+      <c r="AA172">
+        <v>304</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -15616,6 +17170,15 @@
       <c r="X173">
         <v>1.14</v>
       </c>
+      <c r="Y173">
+        <v>-152</v>
+      </c>
+      <c r="Z173">
+        <v>-137</v>
+      </c>
+      <c r="AA173">
+        <v>15</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -15704,6 +17267,15 @@
       <c r="X174">
         <v>1.17</v>
       </c>
+      <c r="Y174">
+        <v>-139</v>
+      </c>
+      <c r="Z174">
+        <v>-75</v>
+      </c>
+      <c r="AA174">
+        <v>64</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -15792,6 +17364,15 @@
       <c r="X175">
         <v>1.33</v>
       </c>
+      <c r="Y175">
+        <v>-509</v>
+      </c>
+      <c r="Z175">
+        <v>-401</v>
+      </c>
+      <c r="AA175">
+        <v>108</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -15880,6 +17461,15 @@
       <c r="X176">
         <v>1.47</v>
       </c>
+      <c r="Y176">
+        <v>-450</v>
+      </c>
+      <c r="Z176">
+        <v>-345</v>
+      </c>
+      <c r="AA176">
+        <v>105</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -15968,6 +17558,15 @@
       <c r="X177">
         <v>1.74</v>
       </c>
+      <c r="Y177">
+        <v>-545</v>
+      </c>
+      <c r="Z177">
+        <v>-326</v>
+      </c>
+      <c r="AA177">
+        <v>219</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -16056,6 +17655,15 @@
       <c r="X178">
         <v>2.19</v>
       </c>
+      <c r="Y178">
+        <v>-522</v>
+      </c>
+      <c r="Z178">
+        <v>-350</v>
+      </c>
+      <c r="AA178">
+        <v>172</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -16144,6 +17752,15 @@
       <c r="X179">
         <v>1.51</v>
       </c>
+      <c r="Y179">
+        <v>-733</v>
+      </c>
+      <c r="Z179">
+        <v>-551</v>
+      </c>
+      <c r="AA179">
+        <v>182</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -16232,6 +17849,15 @@
       <c r="X180">
         <v>1.01</v>
       </c>
+      <c r="Y180">
+        <v>-10</v>
+      </c>
+      <c r="Z180">
+        <v>-8</v>
+      </c>
+      <c r="AA180">
+        <v>2</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -16320,6 +17946,15 @@
       <c r="X181">
         <v>2.31</v>
       </c>
+      <c r="Y181">
+        <v>-603</v>
+      </c>
+      <c r="Z181">
+        <v>-295</v>
+      </c>
+      <c r="AA181">
+        <v>308</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -16408,6 +18043,15 @@
       <c r="X182">
         <v>2.56</v>
       </c>
+      <c r="Y182">
+        <v>-711</v>
+      </c>
+      <c r="Z182">
+        <v>-542</v>
+      </c>
+      <c r="AA182">
+        <v>169</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -16496,6 +18140,15 @@
       <c r="X183">
         <v>4.04</v>
       </c>
+      <c r="Y183">
+        <v>-932</v>
+      </c>
+      <c r="Z183">
+        <v>-674</v>
+      </c>
+      <c r="AA183">
+        <v>258</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -16584,6 +18237,15 @@
       <c r="X184">
         <v>1.71</v>
       </c>
+      <c r="Y184">
+        <v>-419</v>
+      </c>
+      <c r="Z184">
+        <v>-334</v>
+      </c>
+      <c r="AA184">
+        <v>85</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -16672,6 +18334,15 @@
       <c r="X185">
         <v>3.21</v>
       </c>
+      <c r="Y185">
+        <v>-673</v>
+      </c>
+      <c r="Z185">
+        <v>-470</v>
+      </c>
+      <c r="AA185">
+        <v>203</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -16760,6 +18431,15 @@
       <c r="X186">
         <v>1.94</v>
       </c>
+      <c r="Y186">
+        <v>-494</v>
+      </c>
+      <c r="Z186">
+        <v>-391</v>
+      </c>
+      <c r="AA186">
+        <v>103</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -16848,6 +18528,15 @@
       <c r="X187">
         <v>1.86</v>
       </c>
+      <c r="Y187">
+        <v>-546</v>
+      </c>
+      <c r="Z187">
+        <v>-457</v>
+      </c>
+      <c r="AA187">
+        <v>89</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -16936,6 +18625,15 @@
       <c r="X188">
         <v>2.62</v>
       </c>
+      <c r="Y188">
+        <v>-549</v>
+      </c>
+      <c r="Z188">
+        <v>-424</v>
+      </c>
+      <c r="AA188">
+        <v>125</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -17024,6 +18722,15 @@
       <c r="X189">
         <v>1.22</v>
       </c>
+      <c r="Y189">
+        <v>-274</v>
+      </c>
+      <c r="Z189">
+        <v>-167</v>
+      </c>
+      <c r="AA189">
+        <v>107</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -17112,6 +18819,15 @@
       <c r="X190">
         <v>1.49</v>
       </c>
+      <c r="Y190">
+        <v>-208</v>
+      </c>
+      <c r="Z190">
+        <v>-40</v>
+      </c>
+      <c r="AA190">
+        <v>168</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -17200,6 +18916,15 @@
       <c r="X191">
         <v>1.47</v>
       </c>
+      <c r="Y191">
+        <v>-211</v>
+      </c>
+      <c r="Z191">
+        <v>-63</v>
+      </c>
+      <c r="AA191">
+        <v>148</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -17288,6 +19013,15 @@
       <c r="X192">
         <v>1.34</v>
       </c>
+      <c r="Y192">
+        <v>-205</v>
+      </c>
+      <c r="Z192">
+        <v>-81</v>
+      </c>
+      <c r="AA192">
+        <v>124</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -17376,6 +19110,15 @@
       <c r="X193">
         <v>0.91</v>
       </c>
+      <c r="Y193">
+        <v>216</v>
+      </c>
+      <c r="Z193">
+        <v>176</v>
+      </c>
+      <c r="AA193">
+        <v>-40</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -17464,6 +19207,15 @@
       <c r="X194">
         <v>1.38</v>
       </c>
+      <c r="Y194">
+        <v>-153</v>
+      </c>
+      <c r="Z194">
+        <v>-99</v>
+      </c>
+      <c r="AA194">
+        <v>54</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -17552,6 +19304,15 @@
       <c r="X195">
         <v>2.19</v>
       </c>
+      <c r="Y195">
+        <v>-317</v>
+      </c>
+      <c r="Z195">
+        <v>-164</v>
+      </c>
+      <c r="AA195">
+        <v>153</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -17640,6 +19401,15 @@
       <c r="X196">
         <v>1.21</v>
       </c>
+      <c r="Y196">
+        <v>-454</v>
+      </c>
+      <c r="Z196">
+        <v>-386</v>
+      </c>
+      <c r="AA196">
+        <v>68</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -17728,6 +19498,15 @@
       <c r="X197">
         <v>1.25</v>
       </c>
+      <c r="Y197">
+        <v>-166</v>
+      </c>
+      <c r="Z197">
+        <v>-87</v>
+      </c>
+      <c r="AA197">
+        <v>79</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -17816,6 +19595,15 @@
       <c r="X198">
         <v>2.37</v>
       </c>
+      <c r="Y198">
+        <v>-748</v>
+      </c>
+      <c r="Z198">
+        <v>-513</v>
+      </c>
+      <c r="AA198">
+        <v>235</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -17904,6 +19692,15 @@
       <c r="X199">
         <v>1.69</v>
       </c>
+      <c r="Y199">
+        <v>-371</v>
+      </c>
+      <c r="Z199">
+        <v>-278</v>
+      </c>
+      <c r="AA199">
+        <v>93</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -17992,6 +19789,15 @@
       <c r="X200">
         <v>2.39</v>
       </c>
+      <c r="Y200">
+        <v>-838</v>
+      </c>
+      <c r="Z200">
+        <v>-622</v>
+      </c>
+      <c r="AA200">
+        <v>216</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -18080,6 +19886,15 @@
       <c r="X201">
         <v>2.46</v>
       </c>
+      <c r="Y201">
+        <v>-327</v>
+      </c>
+      <c r="Z201">
+        <v>-204</v>
+      </c>
+      <c r="AA201">
+        <v>123</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -18168,6 +19983,15 @@
       <c r="X202">
         <v>2</v>
       </c>
+      <c r="Y202">
+        <v>-445</v>
+      </c>
+      <c r="Z202">
+        <v>-346</v>
+      </c>
+      <c r="AA202">
+        <v>99</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -18256,6 +20080,15 @@
       <c r="X203">
         <v>1.23</v>
       </c>
+      <c r="Y203">
+        <v>-117</v>
+      </c>
+      <c r="Z203">
+        <v>-18</v>
+      </c>
+      <c r="AA203">
+        <v>99</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -18344,6 +20177,15 @@
       <c r="X204">
         <v>2.53</v>
       </c>
+      <c r="Y204">
+        <v>-304</v>
+      </c>
+      <c r="Z204">
+        <v>-197</v>
+      </c>
+      <c r="AA204">
+        <v>107</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -18432,6 +20274,15 @@
       <c r="X205">
         <v>0.9</v>
       </c>
+      <c r="Y205">
+        <v>-97</v>
+      </c>
+      <c r="Z205">
+        <v>-132</v>
+      </c>
+      <c r="AA205">
+        <v>-35</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -18520,6 +20371,15 @@
       <c r="X206">
         <v>1.16</v>
       </c>
+      <c r="Y206">
+        <v>-243</v>
+      </c>
+      <c r="Z206">
+        <v>-211</v>
+      </c>
+      <c r="AA206">
+        <v>32</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -18608,6 +20468,15 @@
       <c r="X207">
         <v>2.27</v>
       </c>
+      <c r="Y207">
+        <v>-681</v>
+      </c>
+      <c r="Z207">
+        <v>-521</v>
+      </c>
+      <c r="AA207">
+        <v>160</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -18696,6 +20565,15 @@
       <c r="X208">
         <v>1.46</v>
       </c>
+      <c r="Y208">
+        <v>-432</v>
+      </c>
+      <c r="Z208">
+        <v>-309</v>
+      </c>
+      <c r="AA208">
+        <v>123</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -18784,6 +20662,15 @@
       <c r="X209">
         <v>2.16</v>
       </c>
+      <c r="Y209">
+        <v>-577</v>
+      </c>
+      <c r="Z209">
+        <v>-306</v>
+      </c>
+      <c r="AA209">
+        <v>271</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -18872,6 +20759,15 @@
       <c r="X210">
         <v>1.52</v>
       </c>
+      <c r="Y210">
+        <v>-249</v>
+      </c>
+      <c r="Z210">
+        <v>-185</v>
+      </c>
+      <c r="AA210">
+        <v>64</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -18959,6 +20855,15 @@
       </c>
       <c r="X211">
         <v>0.23</v>
+      </c>
+      <c r="Y211">
+        <v>297</v>
+      </c>
+      <c r="Z211">
+        <v>203</v>
+      </c>
+      <c r="AA211">
+        <v>-94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished initial markdown report version for KB
</commit_message>
<xml_diff>
--- a/processed_data/joined.xlsx
+++ b/processed_data/joined.xlsx
@@ -675,7 +675,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>no change</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>no change</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
@@ -7218,7 +7218,7 @@
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>no change</t>
         </is>
       </c>
       <c r="W64" t="inlineStr">
@@ -8074,7 +8074,7 @@
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>no change</t>
         </is>
       </c>
       <c r="W72" t="inlineStr">
@@ -10428,7 +10428,7 @@
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>no change</t>
         </is>
       </c>
       <c r="W94" t="inlineStr">
@@ -16639,7 +16639,7 @@
       </c>
       <c r="W152" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>no change</t>
         </is>
       </c>
       <c r="X152">
@@ -17583,7 +17583,7 @@
       </c>
       <c r="R161" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>no change</t>
         </is>
       </c>
       <c r="S161" t="inlineStr">
@@ -19509,7 +19509,7 @@
       </c>
       <c r="R179" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>no change</t>
         </is>
       </c>
       <c r="S179" t="inlineStr">

</xml_diff>